<commit_message>
feat: Summarize the rules and organize the requirements.
</commit_message>
<xml_diff>
--- a/Doc/RulesDiff.xlsx
+++ b/Doc/RulesDiff.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Project\UnrealCppLint\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB79973-90B1-4739-BE1D-60CDE587051A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA3A5E1-15CC-4732-AF40-45976D1F32D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -884,7 +884,7 @@
   <dimension ref="A1:K69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.25" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
feat: Update config file, remove test filter.
</commit_message>
<xml_diff>
--- a/Doc/RulesDiff.xlsx
+++ b/Doc/RulesDiff.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WXDDevelopment\Tools\UnrealCppLint\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Other_Project\UnrealCppLint\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221A7B27-4F5C-4C05-BDC2-55E307489046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3AA4225-ECFA-4215-BC34-319FF2CCD2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5590" yWindow="2600" windowWidth="22990" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="changedlog" sheetId="2" r:id="rId1"/>
@@ -1225,15 +1225,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1457325</xdr:colOff>
+      <xdr:colOff>1381125</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>619125</xdr:rowOff>
+      <xdr:rowOff>650875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2885375</xdr:colOff>
+      <xdr:colOff>2809175</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>152111</xdr:rowOff>
+      <xdr:rowOff>183861</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1256,8 +1256,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13287375" y="619125"/>
-          <a:ext cx="5600000" cy="2314286"/>
+          <a:off x="13204825" y="650875"/>
+          <a:ext cx="5600000" cy="2301586"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1534,20 +1534,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC477204-EF6E-4062-A97C-AC30FA36BBE9}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="41.125" defaultRowHeight="54.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="41.08203125" defaultRowHeight="54.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="37.08203125" style="4" customWidth="1"/>
     <col min="2" max="2" width="77" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.125" style="2"/>
+    <col min="3" max="3" width="41.08203125" style="2"/>
     <col min="4" max="4" width="54.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="41.125" style="16"/>
+    <col min="5" max="16384" width="41.08203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="2" t="s">
         <v>108</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>114</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>115</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>118</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>120</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>125</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>128</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>136</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>135</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>137</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>143</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>144</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>151</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>154</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>157</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>161</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>165</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>169</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>174</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>178</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>179</v>
       </c>
@@ -1838,25 +1838,25 @@
   <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="35.25" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="35.25" defaultRowHeight="15.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.25" style="12" customWidth="1"/>
     <col min="2" max="2" width="13" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68.25" style="2" customWidth="1"/>
     <col min="4" max="4" width="52" style="2" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="35.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="9.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="129.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.08203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="35.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.33203125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="9.58203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="129.58203125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="35.25" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11"/>
       <c r="B1" s="8"/>
       <c r="C1" s="5" t="s">
@@ -1879,7 +1879,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="28" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>6</v>
       </c>
@@ -1902,7 +1902,7 @@
       </c>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:11" ht="57" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="56" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>54</v>
       </c>
@@ -1929,7 +1929,7 @@
       </c>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
       <c r="B4" s="18" t="s">
         <v>57</v>
@@ -1948,7 +1948,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
       <c r="B5" s="18"/>
       <c r="C5" s="6" t="s">
@@ -1965,7 +1965,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="28" x14ac:dyDescent="0.3">
       <c r="A6" s="20"/>
       <c r="B6" s="18" t="s">
         <v>61</v>
@@ -1987,7 +1987,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="28" x14ac:dyDescent="0.3">
       <c r="A7" s="20"/>
       <c r="B7" s="18"/>
       <c r="C7" s="6" t="s">
@@ -2002,7 +2002,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="28" x14ac:dyDescent="0.3">
       <c r="A8" s="20"/>
       <c r="B8" s="18" t="s">
         <v>62</v>
@@ -2019,7 +2019,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21"/>
       <c r="B9" s="18"/>
       <c r="C9" s="6" t="s">
@@ -2032,7 +2032,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="9"/>
       <c r="C10" s="6"/>
@@ -2041,7 +2041,7 @@
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="9"/>
       <c r="C11" s="6"/>
@@ -2050,7 +2050,7 @@
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="9"/>
       <c r="C12" s="6"/>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="G12" s="14"/>
     </row>
-    <row r="20" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>10</v>
       </c>
@@ -2074,7 +2074,7 @@
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A21" s="17"/>
       <c r="B21" s="9"/>
       <c r="C21" s="6" t="s">
@@ -2085,7 +2085,7 @@
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A22" s="17"/>
       <c r="B22" s="9"/>
       <c r="C22" s="6" t="s">
@@ -2098,7 +2098,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A23" s="17"/>
       <c r="B23" s="9"/>
       <c r="C23" s="6" t="s">
@@ -2109,7 +2109,7 @@
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>3</v>
       </c>
@@ -2124,7 +2124,7 @@
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>26</v>
       </c>
@@ -2137,7 +2137,7 @@
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>27</v>
       </c>
@@ -2150,7 +2150,7 @@
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>30</v>
       </c>
@@ -2163,7 +2163,7 @@
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>32</v>
       </c>
@@ -2174,7 +2174,7 @@
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
     </row>
-    <row r="29" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>33</v>
       </c>
@@ -2187,7 +2187,7 @@
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>34</v>
       </c>
@@ -2200,7 +2200,7 @@
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>37</v>
       </c>
@@ -2213,7 +2213,7 @@
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
     </row>
-    <row r="32" spans="1:7" ht="57" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>39</v>
       </c>
@@ -2226,7 +2226,7 @@
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>41</v>
       </c>
@@ -2239,7 +2239,7 @@
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
     </row>
-    <row r="34" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>43</v>
       </c>
@@ -2252,7 +2252,7 @@
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="11"/>
       <c r="B35" s="9"/>
       <c r="C35" s="6" t="s">
@@ -2263,7 +2263,7 @@
       <c r="F35" s="14"/>
       <c r="G35" s="14"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="11"/>
       <c r="B36" s="9"/>
       <c r="C36" s="6" t="s">
@@ -2274,7 +2274,7 @@
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
     </row>
-    <row r="37" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>47</v>
       </c>
@@ -2287,7 +2287,7 @@
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>59</v>
       </c>
@@ -2298,7 +2298,7 @@
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>49</v>
       </c>
@@ -2311,7 +2311,7 @@
       <c r="F39" s="14"/>
       <c r="G39" s="14"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>51</v>
       </c>
@@ -2324,7 +2324,7 @@
       <c r="F40" s="14"/>
       <c r="G40" s="14"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="11"/>
       <c r="B41" s="9"/>
       <c r="C41" s="6" t="s">
@@ -2335,7 +2335,7 @@
       <c r="F41" s="14"/>
       <c r="G41" s="14"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="11"/>
       <c r="B42" s="9"/>
       <c r="C42" s="6"/>
@@ -2344,7 +2344,7 @@
       <c r="F42" s="14"/>
       <c r="G42" s="14"/>
     </row>
-    <row r="43" spans="1:7" ht="313.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="308" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>65</v>
       </c>
@@ -2357,7 +2357,7 @@
       <c r="F43" s="14"/>
       <c r="G43" s="14"/>
     </row>
-    <row r="44" spans="1:7" ht="342" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="322" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>67</v>
       </c>
@@ -2370,7 +2370,7 @@
       <c r="F44" s="14"/>
       <c r="G44" s="14"/>
     </row>
-    <row r="45" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
         <v>69</v>
       </c>
@@ -2383,7 +2383,7 @@
       <c r="F45" s="14"/>
       <c r="G45" s="14"/>
     </row>
-    <row r="46" spans="1:7" ht="327.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="322" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
         <v>71</v>
       </c>
@@ -2396,7 +2396,7 @@
       <c r="F46" s="14"/>
       <c r="G46" s="14"/>
     </row>
-    <row r="47" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A47" s="11"/>
       <c r="B47" s="9"/>
       <c r="C47" s="6" t="s">
@@ -2407,7 +2407,7 @@
       <c r="F47" s="14"/>
       <c r="G47" s="14"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="11"/>
       <c r="B48" s="9"/>
       <c r="C48" s="6" t="s">
@@ -2418,7 +2418,7 @@
       <c r="F48" s="14"/>
       <c r="G48" s="14"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="11"/>
       <c r="B49" s="9"/>
       <c r="C49" s="6" t="s">
@@ -2429,7 +2429,7 @@
       <c r="F49" s="14"/>
       <c r="G49" s="14"/>
     </row>
-    <row r="50" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A50" s="11"/>
       <c r="B50" s="9"/>
       <c r="C50" s="6" t="s">
@@ -2440,7 +2440,7 @@
       <c r="F50" s="14"/>
       <c r="G50" s="14"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
         <v>77</v>
       </c>
@@ -2453,7 +2453,7 @@
       <c r="F51" s="14"/>
       <c r="G51" s="14"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="11"/>
       <c r="B52" s="9"/>
       <c r="C52" s="6" t="s">
@@ -2464,7 +2464,7 @@
       <c r="F52" s="14"/>
       <c r="G52" s="14"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="11"/>
       <c r="B53" s="9"/>
       <c r="C53" s="6" t="s">
@@ -2475,7 +2475,7 @@
       <c r="F53" s="14"/>
       <c r="G53" s="14"/>
     </row>
-    <row r="54" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A54" s="11"/>
       <c r="B54" s="9"/>
       <c r="C54" s="6" t="s">
@@ -2486,7 +2486,7 @@
       <c r="F54" s="14"/>
       <c r="G54" s="14"/>
     </row>
-    <row r="55" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A55" s="11"/>
       <c r="B55" s="9"/>
       <c r="C55" s="6" t="s">
@@ -2497,7 +2497,7 @@
       <c r="F55" s="14"/>
       <c r="G55" s="14"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
         <v>83</v>
       </c>
@@ -2510,7 +2510,7 @@
       <c r="F56" s="14"/>
       <c r="G56" s="14"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="11"/>
       <c r="B57" s="9"/>
       <c r="C57" s="6" t="s">
@@ -2521,7 +2521,7 @@
       <c r="F57" s="14"/>
       <c r="G57" s="14"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
         <v>18</v>
       </c>
@@ -2532,7 +2532,7 @@
       <c r="F58" s="14"/>
       <c r="G58" s="14"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
         <v>19</v>
       </c>
@@ -2543,7 +2543,7 @@
       <c r="F59" s="14"/>
       <c r="G59" s="14"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
         <v>20</v>
       </c>
@@ -2554,7 +2554,7 @@
       <c r="F60" s="14"/>
       <c r="G60" s="14"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
         <v>21</v>
       </c>
@@ -2565,7 +2565,7 @@
       <c r="F61" s="14"/>
       <c r="G61" s="14"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
         <v>22</v>
       </c>
@@ -2576,7 +2576,7 @@
       <c r="F62" s="14"/>
       <c r="G62" s="14"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="11" t="s">
         <v>23</v>
       </c>
@@ -2587,7 +2587,7 @@
       <c r="F63" s="14"/>
       <c r="G63" s="14"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="11" t="s">
         <v>24</v>
       </c>
@@ -2598,7 +2598,7 @@
       <c r="F64" s="14"/>
       <c r="G64" s="14"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="11" t="s">
         <v>25</v>
       </c>
@@ -2609,7 +2609,7 @@
       <c r="F65" s="14"/>
       <c r="G65" s="14"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="11"/>
       <c r="B66" s="9"/>
       <c r="C66" s="6"/>
@@ -2618,7 +2618,7 @@
       <c r="F66" s="14"/>
       <c r="G66" s="14"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="11"/>
       <c r="B67" s="9"/>
       <c r="C67" s="6"/>
@@ -2627,7 +2627,7 @@
       <c r="F67" s="14"/>
       <c r="G67" s="14"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="11"/>
       <c r="B68" s="9"/>
       <c r="C68" s="6"/>

</xml_diff>